<commit_message>
Add to cart test
</commit_message>
<xml_diff>
--- a/github.com/upkarsinghrathaur/AutomationPractice.git/AutomationPractice/src/test/resources/dataFile/testData.xlsx
+++ b/github.com/upkarsinghrathaur/AutomationPractice.git/AutomationPractice/src/test/resources/dataFile/testData.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14145" windowHeight="4605"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14145" windowHeight="3465" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="checkSignIn" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="addToCartProduct" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:J14"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>createEmail</t>
   </si>
@@ -125,6 +125,36 @@
   </si>
   <si>
     <t>Highway</t>
+  </si>
+  <si>
+    <t>accountName</t>
+  </si>
+  <si>
+    <t>cartMessage</t>
+  </si>
+  <si>
+    <t>Product successfully added to your shopping cart</t>
+  </si>
+  <si>
+    <t>Upkar Singh</t>
+  </si>
+  <si>
+    <t>productPrice</t>
+  </si>
+  <si>
+    <t>orderCompleteMessage</t>
+  </si>
+  <si>
+    <t>$27.00</t>
+  </si>
+  <si>
+    <t>totalPrice</t>
+  </si>
+  <si>
+    <t>$29.00</t>
+  </si>
+  <si>
+    <t>Your order on My Store is complete.</t>
   </si>
 </sst>
 </file>
@@ -473,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -606,7 +636,7 @@
         <v>32</v>
       </c>
       <c r="P2">
-        <v>209831</v>
+        <v>20831</v>
       </c>
       <c r="Q2" t="s">
         <v>34</v>
@@ -638,12 +668,55 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added SauceLabs test class
</commit_message>
<xml_diff>
--- a/github.com/upkarsinghrathaur/AutomationPractice.git/AutomationPractice/src/test/resources/dataFile/testData.xlsx
+++ b/github.com/upkarsinghrathaur/AutomationPractice.git/AutomationPractice/src/test/resources/dataFile/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14145" windowHeight="3345" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14145" windowHeight="2055"/>
   </bookViews>
   <sheets>
     <sheet name="checkSignIn" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="deleteCommentTest" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:I9"/>
+  <oleSize ref="A1:I5"/>
 </workbook>
 </file>
 
@@ -524,7 +524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -814,7 +814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>